<commit_message>
correcting m3 layout with 611_hotel connected
</commit_message>
<xml_diff>
--- a/Lehigh_energy_modeling.xlsx
+++ b/Lehigh_energy_modeling.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt2/Documents/NRECA/MicrogridUp/microgridup/Lehigh_loadshapes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt2/Documents/NRECA/MicrogridUp/microgridup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFEF467-ED91-6740-8784-9889C58D954B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650ACE8B-0192-824C-A4CC-5E336CBD637B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{5E54B31A-263E-7345-873B-B53A0B6021F8}"/>
+    <workbookView xWindow="9480" yWindow="-19940" windowWidth="19960" windowHeight="16640" xr2:uid="{5E54B31A-263E-7345-873B-B53A0B6021F8}"/>
   </bookViews>
   <sheets>
-    <sheet name="112320_Lehigh.dss" sheetId="3" r:id="rId1"/>
-    <sheet name="6_build+resid_11032020" sheetId="2" r:id="rId2"/>
-    <sheet name="6_buildings_10282020" sheetId="1" r:id="rId3"/>
+    <sheet name="121620_Lehigh" sheetId="4" r:id="rId1"/>
+    <sheet name="112320_Lehigh.dss" sheetId="3" r:id="rId2"/>
+    <sheet name="6_build+resid_11032020" sheetId="2" r:id="rId3"/>
+    <sheet name="6_buildings_10282020" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="209">
   <si>
     <t>35 units</t>
   </si>
@@ -647,6 +648,69 @@
   </si>
   <si>
     <t>*minimum survived outage is often 0 hours</t>
+  </si>
+  <si>
+    <t>LoadShape column in lehigh_load.csv</t>
+  </si>
+  <si>
+    <t>634a_supermarket</t>
+  </si>
+  <si>
+    <t>634b_supermarket</t>
+  </si>
+  <si>
+    <t>634c_supermarket</t>
+  </si>
+  <si>
+    <t>24-hour operations</t>
+  </si>
+  <si>
+    <t>675a_residential1</t>
+  </si>
+  <si>
+    <t>675b_residential1</t>
+  </si>
+  <si>
+    <t>675c_residential1</t>
+  </si>
+  <si>
+    <t>Residential Building</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Should load at 692 be served by m2?</t>
+  </si>
+  <si>
+    <t>*671 was reworked as 611 to match the outline of the model</t>
+  </si>
+  <si>
+    <t>611_hotel</t>
+  </si>
+  <si>
+    <t>652_med_apartment</t>
+  </si>
+  <si>
+    <t>What is the basis of this load shape?</t>
+  </si>
+  <si>
+    <t>645_warehouse1</t>
+  </si>
+  <si>
+    <t>646_med_office</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Load (kW) as of 12/17/2020 </t>
+  </si>
+  <si>
+    <t>Max Load (kW) as of 12/17/2020</t>
+  </si>
+  <si>
+    <t>Min Load (kW) as of 12/17/2020</t>
+  </si>
+  <si>
+    <t>Max Load (kW)  as per bus loads defined in IEEE13</t>
   </si>
 </sst>
 </file>
@@ -690,12 +754,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -710,7 +798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -726,6 +814,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1039,11 +1131,639 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750EAD6B-E5E2-8641-B4B9-B46AEA633FBD}">
+  <dimension ref="A1:Y24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="7" width="22.5" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
+    <col min="9" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" customWidth="1"/>
+    <col min="12" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="22.5" customWidth="1"/>
+    <col min="15" max="15" width="18.83203125" customWidth="1"/>
+    <col min="16" max="16" width="17.1640625" customWidth="1"/>
+    <col min="17" max="24" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="S3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25">
+      <c r="A4" t="s">
+        <v>149</v>
+      </c>
+      <c r="S4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25">
+      <c r="A5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25">
+      <c r="A6" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
+      <c r="K8" t="s">
+        <v>182</v>
+      </c>
+      <c r="M8">
+        <f>133/331</f>
+        <v>0.40181268882175225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25">
+      <c r="K9" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>136</v>
+      </c>
+      <c r="U9" t="s">
+        <v>142</v>
+      </c>
+      <c r="V9" t="s">
+        <v>186</v>
+      </c>
+      <c r="W9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="48" customHeight="1">
+      <c r="A10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="L10" t="s">
+        <v>89</v>
+      </c>
+      <c r="M10" t="s">
+        <v>90</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="17">
+      <c r="A11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11">
+        <v>634</v>
+      </c>
+      <c r="H11">
+        <v>400</v>
+      </c>
+      <c r="I11">
+        <v>194</v>
+      </c>
+      <c r="J11">
+        <v>334</v>
+      </c>
+      <c r="K11">
+        <v>65</v>
+      </c>
+      <c r="L11">
+        <v>0.1</v>
+      </c>
+      <c r="M11">
+        <v>20</v>
+      </c>
+      <c r="N11" t="s">
+        <v>50</v>
+      </c>
+      <c r="O11">
+        <f>7*24</f>
+        <v>168</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>165</v>
+      </c>
+      <c r="R11" s="2">
+        <v>440</v>
+      </c>
+      <c r="S11" s="2">
+        <v>79</v>
+      </c>
+      <c r="T11" s="2">
+        <v>307</v>
+      </c>
+      <c r="U11">
+        <f>Q11*500+R11*1600+T11*420+S11*840</f>
+        <v>981800</v>
+      </c>
+      <c r="V11" s="2">
+        <v>-1521</v>
+      </c>
+      <c r="W11" s="2">
+        <v>2024</v>
+      </c>
+      <c r="X11">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H12">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25">
+      <c r="A13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" t="s">
+        <v>192</v>
+      </c>
+      <c r="F13" t="s">
+        <v>190</v>
+      </c>
+      <c r="H13">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25">
+      <c r="A14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" t="s">
+        <v>192</v>
+      </c>
+      <c r="F14" t="s">
+        <v>191</v>
+      </c>
+      <c r="H14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="17">
+      <c r="A15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" t="s">
+        <v>164</v>
+      </c>
+      <c r="G15" t="s">
+        <v>198</v>
+      </c>
+      <c r="H15">
+        <v>772.9</v>
+      </c>
+      <c r="I15">
+        <v>312</v>
+      </c>
+      <c r="J15">
+        <v>700</v>
+      </c>
+      <c r="K15">
+        <v>111</v>
+      </c>
+      <c r="L15">
+        <v>0.1</v>
+      </c>
+      <c r="M15">
+        <v>20</v>
+      </c>
+      <c r="N15" t="s">
+        <v>50</v>
+      </c>
+      <c r="O15">
+        <f>7*24</f>
+        <v>168</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q15">
+        <v>265</v>
+      </c>
+      <c r="R15">
+        <v>1234</v>
+      </c>
+      <c r="S15">
+        <v>198</v>
+      </c>
+      <c r="T15">
+        <v>553</v>
+      </c>
+      <c r="U15">
+        <f>Q15*500+R15*1600+T15*420+S15*840</f>
+        <v>2505480</v>
+      </c>
+      <c r="V15">
+        <v>214920</v>
+      </c>
+      <c r="W15">
+        <v>307</v>
+      </c>
+      <c r="X15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25">
+      <c r="A16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" t="s">
+        <v>160</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F16" t="s">
+        <v>193</v>
+      </c>
+      <c r="H16">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="A17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" t="s">
+        <v>161</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F17" t="s">
+        <v>194</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="H17">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24">
+      <c r="A18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F18" t="s">
+        <v>195</v>
+      </c>
+      <c r="H18">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="17">
+      <c r="A19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19">
+        <v>684</v>
+      </c>
+      <c r="H19">
+        <f>170+128</f>
+        <v>298</v>
+      </c>
+      <c r="I19">
+        <v>275</v>
+      </c>
+      <c r="J19" s="13">
+        <v>500</v>
+      </c>
+      <c r="K19">
+        <v>114</v>
+      </c>
+      <c r="L19">
+        <v>0.1</v>
+      </c>
+      <c r="M19">
+        <v>20</v>
+      </c>
+      <c r="N19" t="s">
+        <v>50</v>
+      </c>
+      <c r="O19">
+        <f>7*24</f>
+        <v>168</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q19">
+        <v>81</v>
+      </c>
+      <c r="R19">
+        <v>432</v>
+      </c>
+      <c r="S19">
+        <v>83</v>
+      </c>
+      <c r="T19">
+        <v>225</v>
+      </c>
+      <c r="U19">
+        <f>Q19*500+R19*1600+T19*420+S19*840</f>
+        <v>895920</v>
+      </c>
+      <c r="V19">
+        <v>109888</v>
+      </c>
+      <c r="W19">
+        <v>1067</v>
+      </c>
+      <c r="X19">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
+      <c r="A20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20">
+        <v>611</v>
+      </c>
+      <c r="E20" t="s">
+        <v>176</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="H20">
+        <v>170</v>
+      </c>
+      <c r="I20">
+        <v>200</v>
+      </c>
+      <c r="J20">
+        <v>351</v>
+      </c>
+      <c r="K20">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24">
+      <c r="A21" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21">
+        <v>652</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F21" t="s">
+        <v>201</v>
+      </c>
+      <c r="H21">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" ht="17">
+      <c r="A22" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" t="s">
+        <v>170</v>
+      </c>
+      <c r="C22">
+        <v>632645</v>
+      </c>
+      <c r="D22">
+        <v>646</v>
+      </c>
+      <c r="H22">
+        <v>363</v>
+      </c>
+      <c r="I22">
+        <v>150</v>
+      </c>
+      <c r="J22" s="13">
+        <v>412</v>
+      </c>
+      <c r="K22">
+        <v>26</v>
+      </c>
+      <c r="L22">
+        <v>0.1</v>
+      </c>
+      <c r="M22">
+        <v>20</v>
+      </c>
+      <c r="N22" t="s">
+        <v>50</v>
+      </c>
+      <c r="O22">
+        <f>7*24</f>
+        <v>168</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q22">
+        <v>145</v>
+      </c>
+      <c r="R22">
+        <v>590</v>
+      </c>
+      <c r="S22">
+        <v>98</v>
+      </c>
+      <c r="T22">
+        <v>346</v>
+      </c>
+      <c r="U22">
+        <f>Q22*500+R22*1600+T22*420+S22*840</f>
+        <v>1244140</v>
+      </c>
+      <c r="V22">
+        <v>20343</v>
+      </c>
+      <c r="W22">
+        <v>216</v>
+      </c>
+      <c r="X22">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24">
+      <c r="A23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23">
+        <v>645</v>
+      </c>
+      <c r="E23" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23" t="s">
+        <v>203</v>
+      </c>
+      <c r="H23">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24">
+      <c r="A24" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24">
+        <v>646</v>
+      </c>
+      <c r="E24" t="s">
+        <v>177</v>
+      </c>
+      <c r="F24" t="s">
+        <v>204</v>
+      </c>
+      <c r="H24">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446EF4BD-D0A2-FC45-BEE7-33012DE4E129}">
   <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1642,12 +2362,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C66B282-24B3-4444-829E-2D855F3D6C7A}">
   <dimension ref="A4:O32"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2353,7 +3073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88881737-4936-A046-81BA-9A7BC3A917C0}">
   <dimension ref="A3:W44"/>
   <sheetViews>
@@ -2832,7 +3552,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="2" customFormat="1" ht="68">
+    <row r="35" spans="1:11" s="2" customFormat="1" ht="51">
       <c r="A35" s="2" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
updating loads and print statements for economic analysis
</commit_message>
<xml_diff>
--- a/Lehigh_energy_modeling.xlsx
+++ b/Lehigh_energy_modeling.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt2/Documents/NRECA/MicrogridUp/microgridup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650ACE8B-0192-824C-A4CC-5E336CBD637B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F82FDC-D77E-5C49-A78C-8D1030A9BC4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9480" yWindow="-19940" windowWidth="19960" windowHeight="16640" xr2:uid="{5E54B31A-263E-7345-873B-B53A0B6021F8}"/>
+    <workbookView xWindow="6920" yWindow="700" windowWidth="19960" windowHeight="16640" xr2:uid="{5E54B31A-263E-7345-873B-B53A0B6021F8}"/>
   </bookViews>
   <sheets>
-    <sheet name="121620_Lehigh" sheetId="4" r:id="rId1"/>
-    <sheet name="112320_Lehigh.dss" sheetId="3" r:id="rId2"/>
-    <sheet name="6_build+resid_11032020" sheetId="2" r:id="rId3"/>
-    <sheet name="6_buildings_10282020" sheetId="1" r:id="rId4"/>
+    <sheet name="12222020_Lehigh" sheetId="5" r:id="rId1"/>
+    <sheet name="121620_Lehigh" sheetId="4" r:id="rId2"/>
+    <sheet name="112320_Lehigh.dss" sheetId="3" r:id="rId3"/>
+    <sheet name="6_build+resid_11032020" sheetId="2" r:id="rId4"/>
+    <sheet name="6_buildings_10282020" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="229">
   <si>
     <t>35 units</t>
   </si>
@@ -711,14 +712,75 @@
   </si>
   <si>
     <t>Max Load (kW)  as per bus loads defined in IEEE13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Load (kW) as of 12/22/2020 </t>
+  </si>
+  <si>
+    <t>Max Load (kW) as of 12/22/2020</t>
+  </si>
+  <si>
+    <t>Min Load (kW) as of 12/22/2020</t>
+  </si>
+  <si>
+    <t>*To build the demand_loads for each microgrid, I ran the full model in microgrid.py and pulled the loadshapes from loadShape.csv</t>
+  </si>
+  <si>
+    <t>652_med_apartment Is the basis</t>
+  </si>
+  <si>
+    <t>Res Prob surviving 48 hr outage (%)</t>
+  </si>
+  <si>
+    <t>Start hour of outage</t>
+  </si>
+  <si>
+    <t>CapEx</t>
+  </si>
+  <si>
+    <t>CapEx after incentives</t>
+  </si>
+  <si>
+    <t>Full grid</t>
+  </si>
+  <si>
+    <t>650632'</t>
+  </si>
+  <si>
+    <t>634a_supermarket','634b_supermarket','634c_supermarket','675a_residential1','675b_residential1','675c_residential1','611_hotel','652_med_apartment','645_warehouse1','646_med_office'</t>
+  </si>
+  <si>
+    <t>Critical loads?  All loads in above microgrids, but not the other buses to make the full load of the base</t>
+  </si>
+  <si>
+    <t>TOTALS FOR 4 ISOLATED MICROGRIDS</t>
+  </si>
+  <si>
+    <t>DIFFERENCES</t>
+  </si>
+  <si>
+    <t>Differences between isolated and grouped grid:</t>
+  </si>
+  <si>
+    <t>Totals for 4-isolated microgrids:</t>
+  </si>
+  <si>
+    <t>675a_hospital</t>
+  </si>
+  <si>
+    <t>Similar result in everything but solar, in which the full scale grid needs an additional 300 kW, making it $360k more expensive upfront, but $100k better (less negative) NPV</t>
+  </si>
+  <si>
+    <t>Resilience is much lower than expected: I don't think the Lehigh_reopt/Loadshape.csv is being built correctly, as the loads are way less than the sum of the loads specified in the microgrid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -798,7 +860,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -818,6 +880,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1131,11 +1201,870 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9443FD63-8DC8-B648-8BEF-4F2758B01020}">
+  <dimension ref="A1:AA30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AA15" sqref="AA15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="7" width="22.5" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
+    <col min="9" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" customWidth="1"/>
+    <col min="12" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="22.5" customWidth="1"/>
+    <col min="15" max="15" width="18.83203125" customWidth="1"/>
+    <col min="16" max="16" width="17.1640625" customWidth="1"/>
+    <col min="17" max="26" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S1">
+        <f>24*10</f>
+        <v>240</v>
+      </c>
+      <c r="T1">
+        <f>7*24</f>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="Q2">
+        <f>24*20</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="S3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="S4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="Q6" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="K8" t="s">
+        <v>212</v>
+      </c>
+      <c r="M8">
+        <f>133/331</f>
+        <v>0.40181268882175225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="K9" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>136</v>
+      </c>
+      <c r="U9" t="s">
+        <v>142</v>
+      </c>
+      <c r="V9" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="48" customHeight="1">
+      <c r="A10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="L10" t="s">
+        <v>89</v>
+      </c>
+      <c r="M10" t="s">
+        <v>90</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="X10" t="s">
+        <v>217</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27">
+      <c r="A11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11">
+        <v>634</v>
+      </c>
+      <c r="H11">
+        <v>400</v>
+      </c>
+      <c r="I11">
+        <v>178</v>
+      </c>
+      <c r="J11">
+        <v>306</v>
+      </c>
+      <c r="K11">
+        <v>60</v>
+      </c>
+      <c r="L11">
+        <v>0.08</v>
+      </c>
+      <c r="M11">
+        <v>20</v>
+      </c>
+      <c r="N11" t="s">
+        <v>50</v>
+      </c>
+      <c r="O11">
+        <v>168</v>
+      </c>
+      <c r="P11" s="2">
+        <v>240</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>196</v>
+      </c>
+      <c r="R11" s="2">
+        <v>400</v>
+      </c>
+      <c r="S11" s="2">
+        <v>39</v>
+      </c>
+      <c r="T11" s="2">
+        <v>106</v>
+      </c>
+      <c r="U11" s="15">
+        <f>Q11*500+R11*1600+T11*420+S11*840</f>
+        <v>815280</v>
+      </c>
+      <c r="V11" s="16">
+        <v>-48637</v>
+      </c>
+      <c r="W11" s="16">
+        <v>814580</v>
+      </c>
+      <c r="X11" s="16">
+        <v>508910</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27">
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H12">
+        <v>160</v>
+      </c>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="A13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" t="s">
+        <v>192</v>
+      </c>
+      <c r="F13" t="s">
+        <v>190</v>
+      </c>
+      <c r="H13">
+        <v>120</v>
+      </c>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+    </row>
+    <row r="14" spans="1:27">
+      <c r="A14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" t="s">
+        <v>192</v>
+      </c>
+      <c r="F14" t="s">
+        <v>191</v>
+      </c>
+      <c r="H14">
+        <v>120</v>
+      </c>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+    </row>
+    <row r="15" spans="1:27">
+      <c r="A15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H15">
+        <v>772.9</v>
+      </c>
+      <c r="I15" s="11">
+        <v>430</v>
+      </c>
+      <c r="J15" s="11">
+        <v>700</v>
+      </c>
+      <c r="K15" s="11">
+        <v>111</v>
+      </c>
+      <c r="L15">
+        <v>0.08</v>
+      </c>
+      <c r="M15">
+        <v>20</v>
+      </c>
+      <c r="N15" t="s">
+        <v>50</v>
+      </c>
+      <c r="O15">
+        <v>168</v>
+      </c>
+      <c r="P15" s="2">
+        <v>240</v>
+      </c>
+      <c r="Q15">
+        <v>134</v>
+      </c>
+      <c r="R15">
+        <v>324</v>
+      </c>
+      <c r="S15">
+        <v>43</v>
+      </c>
+      <c r="T15">
+        <v>106</v>
+      </c>
+      <c r="U15" s="15">
+        <f>Q15*500+R15*1600+T15*420+S15*840</f>
+        <v>666040</v>
+      </c>
+      <c r="V15" s="15">
+        <v>10462</v>
+      </c>
+      <c r="W15" s="15">
+        <v>666568</v>
+      </c>
+      <c r="X15" s="15">
+        <v>414147</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>23</v>
+      </c>
+      <c r="AA15" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27">
+      <c r="A16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" t="s">
+        <v>160</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F16" t="s">
+        <v>226</v>
+      </c>
+      <c r="H16">
+        <v>485</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+    </row>
+    <row r="17" spans="1:27">
+      <c r="A17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" t="s">
+        <v>161</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F17" t="s">
+        <v>194</v>
+      </c>
+      <c r="G17" t="s">
+        <v>213</v>
+      </c>
+      <c r="H17">
+        <v>68</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15"/>
+    </row>
+    <row r="18" spans="1:27">
+      <c r="A18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F18" t="s">
+        <v>195</v>
+      </c>
+      <c r="H18">
+        <v>290</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+    </row>
+    <row r="19" spans="1:27">
+      <c r="A19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19">
+        <v>684</v>
+      </c>
+      <c r="H19">
+        <f>170+128</f>
+        <v>298</v>
+      </c>
+      <c r="I19" s="7">
+        <v>145</v>
+      </c>
+      <c r="J19" s="7">
+        <v>270</v>
+      </c>
+      <c r="K19" s="7">
+        <v>60</v>
+      </c>
+      <c r="L19">
+        <v>0.08</v>
+      </c>
+      <c r="M19">
+        <v>20</v>
+      </c>
+      <c r="N19" t="s">
+        <v>50</v>
+      </c>
+      <c r="O19">
+        <v>168</v>
+      </c>
+      <c r="P19" s="2">
+        <v>240</v>
+      </c>
+      <c r="Q19">
+        <v>155</v>
+      </c>
+      <c r="R19">
+        <v>11</v>
+      </c>
+      <c r="S19">
+        <v>20</v>
+      </c>
+      <c r="T19">
+        <v>62</v>
+      </c>
+      <c r="U19" s="15">
+        <f>Q19*500+R19*1600+T19*420+S19*840</f>
+        <v>137940</v>
+      </c>
+      <c r="V19" s="15">
+        <v>-95326</v>
+      </c>
+      <c r="W19" s="15">
+        <v>137677</v>
+      </c>
+      <c r="X19" s="15">
+        <v>119617</v>
+      </c>
+      <c r="Y19" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27">
+      <c r="A20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20">
+        <v>611</v>
+      </c>
+      <c r="E20" t="s">
+        <v>176</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20">
+        <v>170</v>
+      </c>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="2"/>
+    </row>
+    <row r="21" spans="1:27">
+      <c r="A21" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21">
+        <v>652</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F21" t="s">
+        <v>201</v>
+      </c>
+      <c r="H21">
+        <v>128</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="15"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="2"/>
+    </row>
+    <row r="22" spans="1:27">
+      <c r="A22" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" t="s">
+        <v>170</v>
+      </c>
+      <c r="C22">
+        <v>632645</v>
+      </c>
+      <c r="D22">
+        <v>646</v>
+      </c>
+      <c r="H22">
+        <v>363</v>
+      </c>
+      <c r="I22" s="7">
+        <v>139</v>
+      </c>
+      <c r="J22" s="7">
+        <v>384</v>
+      </c>
+      <c r="K22" s="7">
+        <v>25</v>
+      </c>
+      <c r="L22">
+        <v>0.08</v>
+      </c>
+      <c r="M22">
+        <v>20</v>
+      </c>
+      <c r="N22" t="s">
+        <v>50</v>
+      </c>
+      <c r="O22">
+        <v>168</v>
+      </c>
+      <c r="P22" s="2">
+        <v>240</v>
+      </c>
+      <c r="Q22">
+        <v>132</v>
+      </c>
+      <c r="R22">
+        <v>312</v>
+      </c>
+      <c r="S22">
+        <v>57</v>
+      </c>
+      <c r="T22">
+        <v>134</v>
+      </c>
+      <c r="U22" s="15">
+        <f>Q22*500+R22*1600+T22*420+S22*840</f>
+        <v>669360</v>
+      </c>
+      <c r="V22" s="15">
+        <v>-37742</v>
+      </c>
+      <c r="W22" s="15">
+        <v>670106</v>
+      </c>
+      <c r="X22" s="15">
+        <v>420744</v>
+      </c>
+      <c r="Y22" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27">
+      <c r="A23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23">
+        <v>645</v>
+      </c>
+      <c r="E23" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23" t="s">
+        <v>203</v>
+      </c>
+      <c r="H23">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27">
+      <c r="A24" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24">
+        <v>646</v>
+      </c>
+      <c r="E24" t="s">
+        <v>177</v>
+      </c>
+      <c r="F24" t="s">
+        <v>204</v>
+      </c>
+      <c r="H24">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27">
+      <c r="A26" t="s">
+        <v>222</v>
+      </c>
+      <c r="I26">
+        <f>SUM(I11:I24)</f>
+        <v>892</v>
+      </c>
+      <c r="J26">
+        <f>SUM(J11:J24)</f>
+        <v>1660</v>
+      </c>
+      <c r="K26">
+        <f>SUM(K11:K24)</f>
+        <v>256</v>
+      </c>
+      <c r="P26" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" ref="Q26:X26" si="0">SUM(Q11:Q24)</f>
+        <v>617</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="0"/>
+        <v>1047</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="0"/>
+        <v>159</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="0"/>
+        <v>408</v>
+      </c>
+      <c r="U26" s="15">
+        <f t="shared" si="0"/>
+        <v>2288620</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="0"/>
+        <v>-171243</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="0"/>
+        <v>2288931</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="0"/>
+        <v>1463418</v>
+      </c>
+      <c r="Y26">
+        <f>AVERAGE(Y11:Y25)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27">
+      <c r="A28" t="s">
+        <v>218</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="C28" t="s">
+        <v>219</v>
+      </c>
+      <c r="D28">
+        <v>670</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="I28" s="7">
+        <v>626</v>
+      </c>
+      <c r="J28" s="7">
+        <v>1311</v>
+      </c>
+      <c r="K28" s="7">
+        <v>266</v>
+      </c>
+      <c r="L28">
+        <v>0.08</v>
+      </c>
+      <c r="M28">
+        <v>20</v>
+      </c>
+      <c r="N28" t="s">
+        <v>50</v>
+      </c>
+      <c r="O28">
+        <v>168</v>
+      </c>
+      <c r="P28" s="2">
+        <v>240</v>
+      </c>
+      <c r="Q28">
+        <v>570</v>
+      </c>
+      <c r="R28">
+        <v>1378</v>
+      </c>
+      <c r="S28">
+        <v>230</v>
+      </c>
+      <c r="T28">
+        <v>560</v>
+      </c>
+      <c r="U28" s="15">
+        <f>Q28*500+R28*1600+T28*420+S28*840</f>
+        <v>2918200</v>
+      </c>
+      <c r="V28">
+        <v>-72114</v>
+      </c>
+      <c r="W28">
+        <v>2918280</v>
+      </c>
+      <c r="X28">
+        <v>1825515</v>
+      </c>
+      <c r="Y28" s="12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27">
+      <c r="A30" t="s">
+        <v>223</v>
+      </c>
+      <c r="I30">
+        <f>I26-I28</f>
+        <v>266</v>
+      </c>
+      <c r="J30">
+        <f t="shared" ref="J30:K30" si="1">J26-J28</f>
+        <v>349</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="P30" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q30" s="1">
+        <f t="shared" ref="Q30:X30" si="2">Q26-Q28</f>
+        <v>47</v>
+      </c>
+      <c r="R30" s="1">
+        <f t="shared" si="2"/>
+        <v>-331</v>
+      </c>
+      <c r="S30" s="1">
+        <f t="shared" si="2"/>
+        <v>-71</v>
+      </c>
+      <c r="T30" s="1">
+        <f t="shared" si="2"/>
+        <v>-152</v>
+      </c>
+      <c r="U30" s="1">
+        <f t="shared" si="2"/>
+        <v>-629580</v>
+      </c>
+      <c r="V30" s="1">
+        <f t="shared" si="2"/>
+        <v>-99129</v>
+      </c>
+      <c r="W30" s="1">
+        <f t="shared" si="2"/>
+        <v>-629349</v>
+      </c>
+      <c r="X30" s="1">
+        <f t="shared" si="2"/>
+        <v>-362097</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750EAD6B-E5E2-8641-B4B9-B46AEA633FBD}">
   <dimension ref="A1:Y24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1758,12 +2687,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446EF4BD-D0A2-FC45-BEE7-33012DE4E129}">
   <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="D6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2362,7 +3291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C66B282-24B3-4444-829E-2D855F3D6C7A}">
   <dimension ref="A4:O32"/>
   <sheetViews>
@@ -3073,7 +4002,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88881737-4936-A046-81BA-9A7BC3A917C0}">
   <dimension ref="A3:W44"/>
   <sheetViews>

</xml_diff>

<commit_message>
microgrid.py not calculating m2 loads as expected
</commit_message>
<xml_diff>
--- a/Lehigh_energy_modeling.xlsx
+++ b/Lehigh_energy_modeling.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt2/Documents/NRECA/MicrogridUp/microgridup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F82FDC-D77E-5C49-A78C-8D1030A9BC4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4A6AED-20C9-EF4E-8EF0-7CDBCC28A3A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="700" windowWidth="19960" windowHeight="16640" xr2:uid="{5E54B31A-263E-7345-873B-B53A0B6021F8}"/>
+    <workbookView xWindow="-1320" yWindow="-19400" windowWidth="21880" windowHeight="16820" xr2:uid="{5E54B31A-263E-7345-873B-B53A0B6021F8}"/>
   </bookViews>
   <sheets>
-    <sheet name="12222020_Lehigh" sheetId="5" r:id="rId1"/>
-    <sheet name="121620_Lehigh" sheetId="4" r:id="rId2"/>
-    <sheet name="112320_Lehigh.dss" sheetId="3" r:id="rId3"/>
-    <sheet name="6_build+resid_11032020" sheetId="2" r:id="rId4"/>
-    <sheet name="6_buildings_10282020" sheetId="1" r:id="rId5"/>
+    <sheet name="12282020_Lehigh" sheetId="6" r:id="rId1"/>
+    <sheet name="12222020_Lehigh" sheetId="5" r:id="rId2"/>
+    <sheet name="121620_Lehigh" sheetId="4" r:id="rId3"/>
+    <sheet name="112320_Lehigh.dss" sheetId="3" r:id="rId4"/>
+    <sheet name="6_build+resid_11032020" sheetId="2" r:id="rId5"/>
+    <sheet name="6_buildings_10282020" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="229">
   <si>
     <t>35 units</t>
   </si>
@@ -1201,10 +1202,872 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE12C4FF-CFDE-3140-A344-D90A7CE0C361}">
+  <dimension ref="A1:AA30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="7" width="22.5" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
+    <col min="9" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" customWidth="1"/>
+    <col min="12" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="22.5" customWidth="1"/>
+    <col min="15" max="15" width="18.83203125" customWidth="1"/>
+    <col min="16" max="16" width="17.1640625" customWidth="1"/>
+    <col min="17" max="26" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S1">
+        <f>24*10</f>
+        <v>240</v>
+      </c>
+      <c r="T1">
+        <f>7*24</f>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="Q2">
+        <f>24*20</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="S3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="S4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="Q6" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="K8" t="s">
+        <v>212</v>
+      </c>
+      <c r="M8">
+        <f>133/331</f>
+        <v>0.40181268882175225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="K9" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>136</v>
+      </c>
+      <c r="U9" t="s">
+        <v>142</v>
+      </c>
+      <c r="V9" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="48" customHeight="1">
+      <c r="A10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G10" t="s">
+        <v>197</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L10" t="s">
+        <v>89</v>
+      </c>
+      <c r="M10" t="s">
+        <v>90</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="X10" t="s">
+        <v>217</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27">
+      <c r="A11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11">
+        <v>634</v>
+      </c>
+      <c r="H11">
+        <v>400</v>
+      </c>
+      <c r="I11">
+        <v>178</v>
+      </c>
+      <c r="J11">
+        <v>306</v>
+      </c>
+      <c r="K11">
+        <v>60</v>
+      </c>
+      <c r="L11">
+        <v>0.08</v>
+      </c>
+      <c r="M11">
+        <v>20</v>
+      </c>
+      <c r="N11" t="s">
+        <v>50</v>
+      </c>
+      <c r="O11">
+        <v>168</v>
+      </c>
+      <c r="P11" s="2">
+        <v>240</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>196</v>
+      </c>
+      <c r="R11" s="2">
+        <v>400</v>
+      </c>
+      <c r="S11" s="2">
+        <v>39</v>
+      </c>
+      <c r="T11" s="2">
+        <v>106</v>
+      </c>
+      <c r="U11" s="15">
+        <f>Q11*500+R11*1600+T11*420+S11*840</f>
+        <v>815280</v>
+      </c>
+      <c r="V11" s="16">
+        <v>-48637</v>
+      </c>
+      <c r="W11" s="16">
+        <v>814580</v>
+      </c>
+      <c r="X11" s="16">
+        <v>508910</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27">
+      <c r="A12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H12">
+        <v>160</v>
+      </c>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="A13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" t="s">
+        <v>192</v>
+      </c>
+      <c r="F13" t="s">
+        <v>190</v>
+      </c>
+      <c r="H13">
+        <v>120</v>
+      </c>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+    </row>
+    <row r="14" spans="1:27">
+      <c r="A14" t="s">
+        <v>131</v>
+      </c>
+      <c r="B14" t="s">
+        <v>157</v>
+      </c>
+      <c r="E14" t="s">
+        <v>192</v>
+      </c>
+      <c r="F14" t="s">
+        <v>191</v>
+      </c>
+      <c r="H14">
+        <v>120</v>
+      </c>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+    </row>
+    <row r="15" spans="1:27">
+      <c r="A15" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H15">
+        <v>772.9</v>
+      </c>
+      <c r="I15" s="11">
+        <v>163</v>
+      </c>
+      <c r="J15" s="11">
+        <v>389</v>
+      </c>
+      <c r="K15" s="11">
+        <v>53</v>
+      </c>
+      <c r="L15">
+        <v>0.08</v>
+      </c>
+      <c r="M15">
+        <v>20</v>
+      </c>
+      <c r="N15" t="s">
+        <v>50</v>
+      </c>
+      <c r="O15">
+        <v>168</v>
+      </c>
+      <c r="P15" s="2">
+        <v>240</v>
+      </c>
+      <c r="Q15">
+        <v>134</v>
+      </c>
+      <c r="R15">
+        <v>324</v>
+      </c>
+      <c r="S15">
+        <v>43</v>
+      </c>
+      <c r="T15">
+        <v>106</v>
+      </c>
+      <c r="U15" s="15">
+        <f>Q15*500+R15*1600+T15*420+S15*840</f>
+        <v>666040</v>
+      </c>
+      <c r="V15" s="15">
+        <v>10462</v>
+      </c>
+      <c r="W15" s="15">
+        <v>666568</v>
+      </c>
+      <c r="X15" s="15">
+        <v>414147</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>23</v>
+      </c>
+      <c r="AA15" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27">
+      <c r="A16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" t="s">
+        <v>160</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F16" t="s">
+        <v>226</v>
+      </c>
+      <c r="H16">
+        <v>485</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+    </row>
+    <row r="17" spans="1:27">
+      <c r="A17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" t="s">
+        <v>161</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F17" t="s">
+        <v>194</v>
+      </c>
+      <c r="G17" t="s">
+        <v>213</v>
+      </c>
+      <c r="H17">
+        <v>68</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15"/>
+    </row>
+    <row r="18" spans="1:27">
+      <c r="A18" t="s">
+        <v>158</v>
+      </c>
+      <c r="B18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F18" t="s">
+        <v>195</v>
+      </c>
+      <c r="H18">
+        <v>290</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+    </row>
+    <row r="19" spans="1:27">
+      <c r="A19" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19">
+        <v>684</v>
+      </c>
+      <c r="H19">
+        <f>170+128</f>
+        <v>298</v>
+      </c>
+      <c r="I19" s="7">
+        <v>145</v>
+      </c>
+      <c r="J19" s="7">
+        <v>270</v>
+      </c>
+      <c r="K19" s="7">
+        <v>60</v>
+      </c>
+      <c r="L19">
+        <v>0.08</v>
+      </c>
+      <c r="M19">
+        <v>20</v>
+      </c>
+      <c r="N19" t="s">
+        <v>50</v>
+      </c>
+      <c r="O19">
+        <v>168</v>
+      </c>
+      <c r="P19" s="2">
+        <v>240</v>
+      </c>
+      <c r="Q19">
+        <v>155</v>
+      </c>
+      <c r="R19">
+        <v>11</v>
+      </c>
+      <c r="S19">
+        <v>20</v>
+      </c>
+      <c r="T19">
+        <v>62</v>
+      </c>
+      <c r="U19" s="15">
+        <f>Q19*500+R19*1600+T19*420+S19*840</f>
+        <v>137940</v>
+      </c>
+      <c r="V19" s="15">
+        <v>-95326</v>
+      </c>
+      <c r="W19" s="15">
+        <v>137677</v>
+      </c>
+      <c r="X19" s="15">
+        <v>119617</v>
+      </c>
+      <c r="Y19" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27">
+      <c r="A20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20">
+        <v>611</v>
+      </c>
+      <c r="E20" t="s">
+        <v>176</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20">
+        <v>170</v>
+      </c>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="2"/>
+    </row>
+    <row r="21" spans="1:27">
+      <c r="A21" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21">
+        <v>652</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F21" t="s">
+        <v>201</v>
+      </c>
+      <c r="H21">
+        <v>128</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="15"/>
+      <c r="W21" s="15"/>
+      <c r="X21" s="15"/>
+      <c r="Y21" s="2"/>
+    </row>
+    <row r="22" spans="1:27">
+      <c r="A22" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" t="s">
+        <v>170</v>
+      </c>
+      <c r="C22">
+        <v>632645</v>
+      </c>
+      <c r="D22">
+        <v>646</v>
+      </c>
+      <c r="H22">
+        <v>363</v>
+      </c>
+      <c r="I22" s="7">
+        <v>139</v>
+      </c>
+      <c r="J22" s="7">
+        <v>384</v>
+      </c>
+      <c r="K22" s="7">
+        <v>25</v>
+      </c>
+      <c r="L22">
+        <v>0.08</v>
+      </c>
+      <c r="M22">
+        <v>20</v>
+      </c>
+      <c r="N22" t="s">
+        <v>50</v>
+      </c>
+      <c r="O22">
+        <v>168</v>
+      </c>
+      <c r="P22" s="2">
+        <v>240</v>
+      </c>
+      <c r="Q22">
+        <v>132</v>
+      </c>
+      <c r="R22">
+        <v>312</v>
+      </c>
+      <c r="S22">
+        <v>57</v>
+      </c>
+      <c r="T22">
+        <v>134</v>
+      </c>
+      <c r="U22" s="15">
+        <f>Q22*500+R22*1600+T22*420+S22*840</f>
+        <v>669360</v>
+      </c>
+      <c r="V22" s="15">
+        <v>-37742</v>
+      </c>
+      <c r="W22" s="15">
+        <v>670106</v>
+      </c>
+      <c r="X22" s="15">
+        <v>420744</v>
+      </c>
+      <c r="Y22" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27">
+      <c r="A23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23">
+        <v>645</v>
+      </c>
+      <c r="E23" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23" t="s">
+        <v>203</v>
+      </c>
+      <c r="H23">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27">
+      <c r="A24" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24">
+        <v>646</v>
+      </c>
+      <c r="E24" t="s">
+        <v>177</v>
+      </c>
+      <c r="F24" t="s">
+        <v>204</v>
+      </c>
+      <c r="H24">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27">
+      <c r="A26" t="s">
+        <v>222</v>
+      </c>
+      <c r="I26">
+        <f>SUM(I11:I24)</f>
+        <v>625</v>
+      </c>
+      <c r="J26">
+        <f>SUM(J11:J24)</f>
+        <v>1349</v>
+      </c>
+      <c r="K26">
+        <f>SUM(K11:K24)</f>
+        <v>198</v>
+      </c>
+      <c r="P26" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" ref="Q26:X26" si="0">SUM(Q11:Q24)</f>
+        <v>617</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="0"/>
+        <v>1047</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="0"/>
+        <v>159</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="0"/>
+        <v>408</v>
+      </c>
+      <c r="U26" s="15">
+        <f t="shared" si="0"/>
+        <v>2288620</v>
+      </c>
+      <c r="V26">
+        <f t="shared" si="0"/>
+        <v>-171243</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="0"/>
+        <v>2288931</v>
+      </c>
+      <c r="X26">
+        <f t="shared" si="0"/>
+        <v>1463418</v>
+      </c>
+      <c r="Y26">
+        <f>AVERAGE(Y11:Y25)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27">
+      <c r="A28" t="s">
+        <v>218</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="C28" t="s">
+        <v>219</v>
+      </c>
+      <c r="D28">
+        <v>670</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="I28" s="7">
+        <v>626</v>
+      </c>
+      <c r="J28" s="7">
+        <v>1311</v>
+      </c>
+      <c r="K28" s="7">
+        <v>266</v>
+      </c>
+      <c r="L28">
+        <v>0.08</v>
+      </c>
+      <c r="M28">
+        <v>20</v>
+      </c>
+      <c r="N28" t="s">
+        <v>50</v>
+      </c>
+      <c r="O28">
+        <v>168</v>
+      </c>
+      <c r="P28" s="2">
+        <v>240</v>
+      </c>
+      <c r="Q28">
+        <v>570</v>
+      </c>
+      <c r="R28">
+        <v>1378</v>
+      </c>
+      <c r="S28">
+        <v>230</v>
+      </c>
+      <c r="T28">
+        <v>560</v>
+      </c>
+      <c r="U28" s="15">
+        <f>Q28*500+R28*1600+T28*420+S28*840</f>
+        <v>2918200</v>
+      </c>
+      <c r="V28">
+        <v>-72114</v>
+      </c>
+      <c r="W28">
+        <v>2918280</v>
+      </c>
+      <c r="X28">
+        <v>1825515</v>
+      </c>
+      <c r="Y28" s="12">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27">
+      <c r="A30" t="s">
+        <v>223</v>
+      </c>
+      <c r="I30">
+        <f>I26-I28</f>
+        <v>-1</v>
+      </c>
+      <c r="J30">
+        <f t="shared" ref="J30:K30" si="1">J26-J28</f>
+        <v>38</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="1"/>
+        <v>-68</v>
+      </c>
+      <c r="P30" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q30" s="1">
+        <f t="shared" ref="Q30:X30" si="2">Q26-Q28</f>
+        <v>47</v>
+      </c>
+      <c r="R30" s="1">
+        <f t="shared" si="2"/>
+        <v>-331</v>
+      </c>
+      <c r="S30" s="1">
+        <f t="shared" si="2"/>
+        <v>-71</v>
+      </c>
+      <c r="T30" s="1">
+        <f t="shared" si="2"/>
+        <v>-152</v>
+      </c>
+      <c r="U30" s="1">
+        <f t="shared" si="2"/>
+        <v>-629580</v>
+      </c>
+      <c r="V30" s="1">
+        <f t="shared" si="2"/>
+        <v>-99129</v>
+      </c>
+      <c r="W30" s="1">
+        <f t="shared" si="2"/>
+        <v>-629349</v>
+      </c>
+      <c r="X30" s="1">
+        <f t="shared" si="2"/>
+        <v>-362097</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9443FD63-8DC8-B648-8BEF-4F2758B01020}">
   <dimension ref="A1:AA30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
@@ -2059,7 +2922,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750EAD6B-E5E2-8641-B4B9-B46AEA633FBD}">
   <dimension ref="A1:Y24"/>
   <sheetViews>
@@ -2687,7 +3550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446EF4BD-D0A2-FC45-BEE7-33012DE4E129}">
   <dimension ref="A1:W24"/>
   <sheetViews>
@@ -3291,7 +4154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C66B282-24B3-4444-829E-2D855F3D6C7A}">
   <dimension ref="A4:O32"/>
   <sheetViews>
@@ -4002,7 +4865,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88881737-4936-A046-81BA-9A7BC3A917C0}">
   <dimension ref="A3:W44"/>
   <sheetViews>

</xml_diff>